<commit_message>
With translation sentiment multi text class
</commit_message>
<xml_diff>
--- a/inputFiles/Segmentation.xlsx
+++ b/inputFiles/Segmentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyndonchan/languageAzure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviragsrivastava/Downloads/GitHub/languageAzure/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85F92B4-51D5-A043-978A-BBBA614619C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4896D1AA-8774-0A4D-B15F-ECE02CD819D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{97733F8E-00A3-E143-999F-9CB389F936C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{97733F8E-00A3-E143-999F-9CB389F936C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Text</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>Thai food is good, but I prefer Indian cuisine.</t>
-  </si>
-  <si>
-    <t>$</t>
   </si>
 </sst>
 </file>
@@ -257,9 +254,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +574,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,253 +583,253 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
@@ -876,10 +872,7 @@
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="E58" t="s">
-        <v>60</v>
-      </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">

</xml_diff>